<commit_message>
Adding playground for code testing
</commit_message>
<xml_diff>
--- a/Data_files/Suicide-rates-ages-15-17-and-18-24_2015.xlsx
+++ b/Data_files/Suicide-rates-ages-15-17-and-18-24_2015.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marik\Documents\UCDavis_Data_Analytics\Project 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel James Ardoin\Documents\Suicide_Data_Project\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E8FDBF9-E8F9-455C-8DAE-63F93EBAD473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E081F2-E04D-43E0-ABA0-20D94534D55C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suicide 18-24" sheetId="9" r:id="rId1"/>
@@ -771,17 +771,17 @@
   </sheetPr>
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.90625" customWidth="1"/>
-    <col min="2" max="16" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="16" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>18</v>
       </c>
@@ -802,7 +802,7 @@
       <c r="P1" s="25"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -853,7 +853,7 @@
       </c>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -904,7 +904,7 @@
       </c>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>8</v>
       </c>
@@ -925,7 +925,7 @@
       <c r="P4" s="26"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>1</v>
       </c>
@@ -976,7 +976,7 @@
       </c>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>2</v>
       </c>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
@@ -1048,7 +1048,7 @@
       <c r="P7" s="26"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>3</v>
       </c>
@@ -1099,7 +1099,7 @@
       </c>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>4</v>
       </c>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>5</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>6</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>7</v>
       </c>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>10</v>
       </c>
@@ -1324,7 +1324,7 @@
       <c r="P13" s="26"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>3</v>
       </c>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>4</v>
       </c>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>5</v>
       </c>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>6</v>
       </c>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>7</v>
       </c>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>11</v>
       </c>
@@ -1600,7 +1600,7 @@
       <c r="P19" s="26"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>3</v>
       </c>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>4</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>5</v>
       </c>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>6</v>
       </c>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>7</v>
       </c>
@@ -1855,7 +1855,7 @@
       </c>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>14</v>
       </c>
@@ -1878,7 +1878,7 @@
       <c r="R25" s="13"/>
       <c r="S25" s="13"/>
     </row>
-    <row r="26" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>22</v>
       </c>
@@ -1901,7 +1901,7 @@
       <c r="R26" s="13"/>
       <c r="S26" s="13"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>12</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="R27" s="13"/>
       <c r="S27" s="13"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1945,7 +1945,7 @@
       <c r="R28" s="13"/>
       <c r="S28" s="13"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1964,7 +1964,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1983,7 +1983,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2002,7 +2002,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2021,7 +2021,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2040,7 +2040,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2059,7 +2059,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2078,7 +2078,7 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2097,7 +2097,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2116,7 +2116,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2135,7 +2135,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2154,7 +2154,7 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2173,7 +2173,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2192,7 +2192,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2211,7 +2211,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2230,7 +2230,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2249,7 +2249,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2268,7 +2268,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2287,7 +2287,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2306,7 +2306,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2325,7 +2325,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2344,7 +2344,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2363,7 +2363,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2382,7 +2382,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2401,7 +2401,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2420,7 +2420,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2439,7 +2439,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2458,7 +2458,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2477,7 +2477,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2496,7 +2496,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2538,17 +2538,17 @@
   </sheetPr>
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.36328125" customWidth="1"/>
-    <col min="2" max="16" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="16" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
@@ -2568,7 +2568,7 @@
       <c r="O1" s="27"/>
       <c r="P1" s="27"/>
     </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>0.201652</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>8</v>
       </c>
@@ -2688,7 +2688,7 @@
       <c r="O4" s="26"/>
       <c r="P4" s="26"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>1</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>0.35486499999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>2</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>0.178422</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
@@ -2808,7 +2808,7 @@
       <c r="O7" s="26"/>
       <c r="P7" s="26"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>3</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>0.29466999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>4</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>0.42251</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>5</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>0.35056999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>6</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>0.69738</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>7</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>1.98437</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>10</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="O13" s="26"/>
       <c r="P13" s="26"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>3</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>0.52099799999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>4</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>0.76207899999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>5</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>0.59763599999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>6</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>1.2244489999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>7</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>3.3900950000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>11</v>
       </c>
@@ -3348,7 +3348,7 @@
       <c r="O19" s="26"/>
       <c r="P19" s="26"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>3</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>0.25725399999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>4</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>0.35272999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>5</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>0.33207999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>6</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>0.64235900000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>7</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>1.9279120000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>16</v>
       </c>
@@ -3618,7 +3618,7 @@
       <c r="O25" s="28"/>
       <c r="P25" s="28"/>
     </row>
-    <row r="26" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
         <v>12</v>
       </c>
@@ -3638,7 +3638,7 @@
       <c r="O26" s="26"/>
       <c r="P26" s="26"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3678,17 +3678,17 @@
   </sheetPr>
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
-    <col min="2" max="16" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="16" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="18" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
@@ -3709,7 +3709,7 @@
       <c r="P1" s="25"/>
       <c r="Q1" s="14"/>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -3811,7 +3811,7 @@
       </c>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>8</v>
       </c>
@@ -3832,7 +3832,7 @@
       <c r="P4" s="26"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>1</v>
       </c>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>2</v>
       </c>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
@@ -3955,7 +3955,7 @@
       <c r="P7" s="26"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>3</v>
       </c>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>4</v>
       </c>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>5</v>
       </c>
@@ -4108,7 +4108,7 @@
       </c>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>6</v>
       </c>
@@ -4159,7 +4159,7 @@
       </c>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>7</v>
       </c>
@@ -4210,7 +4210,7 @@
       </c>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>10</v>
       </c>
@@ -4231,7 +4231,7 @@
       <c r="P13" s="26"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>3</v>
       </c>
@@ -4282,7 +4282,7 @@
       </c>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>4</v>
       </c>
@@ -4333,7 +4333,7 @@
       </c>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>5</v>
       </c>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>6</v>
       </c>
@@ -4435,7 +4435,7 @@
       </c>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>7</v>
       </c>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>11</v>
       </c>
@@ -4507,7 +4507,7 @@
       <c r="P19" s="26"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>3</v>
       </c>
@@ -4558,7 +4558,7 @@
       </c>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>4</v>
       </c>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>5</v>
       </c>
@@ -4660,7 +4660,7 @@
       </c>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>6</v>
       </c>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>7</v>
       </c>
@@ -4762,7 +4762,7 @@
       </c>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>14</v>
       </c>
@@ -4783,7 +4783,7 @@
       <c r="P25" s="24"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="1:17" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>22</v>
       </c>
@@ -4804,7 +4804,7 @@
       <c r="P26" s="23"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>12</v>
       </c>
@@ -4825,7 +4825,7 @@
       <c r="P27" s="24"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -4844,7 +4844,7 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -4890,13 +4890,13 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6328125" customWidth="1"/>
-    <col min="2" max="16" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="16" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="18" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="18" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
         <v>21</v>
       </c>
@@ -4916,7 +4916,7 @@
       <c r="O1" s="31"/>
       <c r="P1" s="31"/>
     </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>17</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>0.233847</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
@@ -5036,7 +5036,7 @@
       <c r="O4" s="32"/>
       <c r="P4" s="32"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>1</v>
       </c>
@@ -5086,7 +5086,7 @@
         <v>0.391488</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>2</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>0.24696599999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>9</v>
       </c>
@@ -5156,7 +5156,7 @@
       <c r="O7" s="32"/>
       <c r="P7" s="32"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>3</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>0.34715600000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>4</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>0.47127000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>5</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>0.38291500000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>6</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>0.74410500000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>7</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>2.5465840000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>10</v>
       </c>
@@ -5426,7 +5426,7 @@
       <c r="O13" s="32"/>
       <c r="P13" s="32"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>3</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>0.58679999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>4</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>0.81675799999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>5</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>0.59115899999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>6</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>7</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>4.2472560000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>11</v>
       </c>
@@ -5696,7 +5696,7 @@
       <c r="O19" s="32"/>
       <c r="P19" s="32"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>3</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>0.35498600000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>4</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>5</v>
       </c>
@@ -5846,7 +5846,7 @@
         <v>0.48004200000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>6</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>7</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>16</v>
       </c>
@@ -5966,7 +5966,7 @@
       <c r="O25" s="29"/>
       <c r="P25" s="29"/>
     </row>
-    <row r="26" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>12</v>
       </c>
@@ -5986,7 +5986,7 @@
       <c r="O26" s="30"/>
       <c r="P26" s="30"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -6004,7 +6004,7 @@
       <c r="O27" s="13"/>
       <c r="P27" s="13"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>

</xml_diff>